<commit_message>
Add column name to parquet table. Misc cleanup.
</commit_message>
<xml_diff>
--- a/binding_template.xlsx
+++ b/binding_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/hoxa/monument/code/PacmanDev/arrow/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/hoxa/monument/code/JPackageDev/arrow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D354602-5B25-714A-BD91-D160CC7BCF7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE844A9-413F-6545-B517-E7133DEC2325}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="1800" windowWidth="32640" windowHeight="22180" xr2:uid="{EC42FF9A-BE4D-5643-BF37-3334470458AB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12127" uniqueCount="6350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12147" uniqueCount="6370">
   <si>
     <t>NB. =========================================================</t>
   </si>
@@ -19079,6 +19079,66 @@
   </si>
   <si>
     <t>garrow_cuda_buffer_output_stream_set_buffer_size(GArrowCUDABufferOutputStream *stream, gint64 size, GError **error);</t>
+  </si>
+  <si>
+    <t>garrow_cuda_device_manager_new (GError **error);GArrowCUDADeviceManager *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_device_manager_get_context(GArrowCUDADeviceManager *manager, gint gpu_number, GError **error);GArrowCUDAContext *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_device_manager_get_n_devices(GArrowCUDADeviceManager *manager);gsize</t>
+  </si>
+  <si>
+    <t>garrow_cuda_context_get_allocated_size(GArrowCUDAContext *context);gint64</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_new (GArrowCUDAContext *context,gint64 size,GError **error);GArrowCUDABuffer *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_new_ipc (GArrowCUDAContext *context,    GArrowCUDAIPCMemoryHandle *handle,    GError **error);GArrowCUDABuffer *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_new_record_batch (GArrowCUDAContext *context,      GArrowRecordBatch *record_batch,      GError **error);GArrowCUDABuffer *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_copy_to_host (GArrowCUDABuffer *buffer,  gint64 position,  gint64 size,  GError **error);GBytes *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_copy_from_host (GArrowCUDABuffer *buffer,    const guint8 *data,    gint64 size,    GError **error);gboolean</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_export (GArrowCUDABuffer *buffer,   GError **error);GArrowCUDAIPCMemoryHandle *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_get_context (GArrowCUDABuffer *buffer);GArrowCUDAContext *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_read_record_batch (GArrowCUDABuffer *buffer,       GArrowSchema *schema,       GArrowReadOptions *options,       GError **error);GArrowRecordBatch *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_host_buffer_new (gint gpu_number,     gint64 size,     GError **error);GArrowCUDAHostBuffer *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_ipc_memory_handle_new (const guint8 *data,    gsize size,    GError **error);GArrowCUDAIPCMemoryHandle *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_ipc_memory_handle_serialize(GArrowCUDAIPCMemoryHandle *handle, GError **error);GArrowBuffer *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_input_stream_new (GArrowCUDABuffer *buffer);GArrowCUDABufferInputStream *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_output_stream_new (GArrowCUDABuffer *buffer);GArrowCUDABufferOutputStream *</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_output_stream_set_buffer_size(GArrowCUDABufferOutputStream *stream, gint64 size, GError **error);gboolean</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_output_stream_get_buffer_size(GArrowCUDABufferOutputStream *stream);gint64</t>
+  </si>
+  <si>
+    <t>garrow_cuda_buffer_output_stream_get_buffered_size(GArrowCUDABufferOutputStream *stream);gint64</t>
   </si>
 </sst>
 </file>
@@ -19457,8 +19517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FED902-EB18-0343-AD72-2B44E47DC872}">
   <dimension ref="A1:G1777"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1739" workbookViewId="0">
-      <selection activeCell="E1755" sqref="E1755:E1777"/>
+    <sheetView tabSelected="1" topLeftCell="D1750" workbookViewId="0">
+      <selection activeCell="E1765" sqref="E1765"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43718,9 +43778,8 @@
       <c r="C1758" t="s">
         <v>6330</v>
       </c>
-      <c r="E1758" t="str">
-        <f>C1758&amp;";"&amp;B1758</f>
-        <v>garrow_cuda_device_manager_new (GError **error);GArrowCUDADeviceManager *</v>
+      <c r="E1758" t="s">
+        <v>6350</v>
       </c>
     </row>
     <row r="1759" spans="1:5" x14ac:dyDescent="0.2">
@@ -43733,9 +43792,8 @@
       <c r="C1759" t="s">
         <v>6338</v>
       </c>
-      <c r="E1759" t="str">
-        <f t="shared" ref="E1759:E1777" si="0">C1759&amp;";"&amp;B1759</f>
-        <v>garrow_cuda_device_manager_get_context(GArrowCUDADeviceManager *manager, gint gpu_number, GError **error);;GArrowCUDAContext *</v>
+      <c r="E1759" t="s">
+        <v>6351</v>
       </c>
     </row>
     <row r="1760" spans="1:5" x14ac:dyDescent="0.2">
@@ -43748,9 +43806,8 @@
       <c r="C1760" t="s">
         <v>6334</v>
       </c>
-      <c r="E1760" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_device_manager_get_n_devices(GArrowCUDADeviceManager *manager);;gsize</v>
+      <c r="E1760" t="s">
+        <v>6352</v>
       </c>
     </row>
     <row r="1761" spans="1:5" x14ac:dyDescent="0.2">
@@ -43763,9 +43820,8 @@
       <c r="C1761" t="s">
         <v>6335</v>
       </c>
-      <c r="E1761" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_context_get_allocated_size(GArrowCUDAContext *context);;gint64</v>
+      <c r="E1761" t="s">
+        <v>6353</v>
       </c>
     </row>
     <row r="1762" spans="1:5" x14ac:dyDescent="0.2">
@@ -43778,9 +43834,8 @@
       <c r="C1762" t="s">
         <v>6339</v>
       </c>
-      <c r="E1762" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_new (GArrowCUDAContext *context,gint64 size,GError **error);;GArrowCUDABuffer *</v>
+      <c r="E1762" t="s">
+        <v>6354</v>
       </c>
     </row>
     <row r="1763" spans="1:5" x14ac:dyDescent="0.2">
@@ -43793,9 +43848,8 @@
       <c r="C1763" t="s">
         <v>6340</v>
       </c>
-      <c r="E1763" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_new_ipc (GArrowCUDAContext *context,    GArrowCUDAIPCMemoryHandle *handle,    GError **error);;GArrowCUDABuffer *</v>
+      <c r="E1763" t="s">
+        <v>6355</v>
       </c>
     </row>
     <row r="1764" spans="1:5" x14ac:dyDescent="0.2">
@@ -43808,9 +43862,8 @@
       <c r="C1764" t="s">
         <v>6341</v>
       </c>
-      <c r="E1764" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_new_record_batch (GArrowCUDAContext *context,      GArrowRecordBatch *record_batch,      GError **error);;GArrowCUDABuffer *</v>
+      <c r="E1764" t="s">
+        <v>6356</v>
       </c>
     </row>
     <row r="1765" spans="1:5" x14ac:dyDescent="0.2">
@@ -43823,9 +43876,8 @@
       <c r="C1765" t="s">
         <v>6342</v>
       </c>
-      <c r="E1765" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_copy_to_host (GArrowCUDABuffer *buffer,  gint64 position,  gint64 size,  GError **error);;GBytes *</v>
+      <c r="E1765" t="s">
+        <v>6357</v>
       </c>
     </row>
     <row r="1766" spans="1:5" x14ac:dyDescent="0.2">
@@ -43838,9 +43890,8 @@
       <c r="C1766" t="s">
         <v>6343</v>
       </c>
-      <c r="E1766" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_copy_from_host (GArrowCUDABuffer *buffer,    const guint8 *data,    gint64 size,    GError **error);;gboolean</v>
+      <c r="E1766" t="s">
+        <v>6358</v>
       </c>
     </row>
     <row r="1767" spans="1:5" x14ac:dyDescent="0.2">
@@ -43853,9 +43904,8 @@
       <c r="C1767" t="s">
         <v>6344</v>
       </c>
-      <c r="E1767" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_export (GArrowCUDABuffer *buffer,   GError **error);;GArrowCUDAIPCMemoryHandle *</v>
+      <c r="E1767" t="s">
+        <v>6359</v>
       </c>
     </row>
     <row r="1768" spans="1:5" x14ac:dyDescent="0.2">
@@ -43868,9 +43918,8 @@
       <c r="C1768" t="s">
         <v>6331</v>
       </c>
-      <c r="E1768" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_get_context (GArrowCUDABuffer *buffer);;GArrowCUDAContext *</v>
+      <c r="E1768" t="s">
+        <v>6360</v>
       </c>
     </row>
     <row r="1769" spans="1:5" x14ac:dyDescent="0.2">
@@ -43883,9 +43932,8 @@
       <c r="C1769" t="s">
         <v>6345</v>
       </c>
-      <c r="E1769" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_read_record_batch (GArrowCUDABuffer *buffer,       GArrowSchema *schema,       GArrowReadOptions *options,       GError **error);;GArrowRecordBatch *</v>
+      <c r="E1769" t="s">
+        <v>6361</v>
       </c>
     </row>
     <row r="1770" spans="1:5" x14ac:dyDescent="0.2">
@@ -43898,9 +43946,8 @@
       <c r="C1770" t="s">
         <v>6346</v>
       </c>
-      <c r="E1770" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_host_buffer_new (gint gpu_number,     gint64 size,     GError **error);;GArrowCUDAHostBuffer *</v>
+      <c r="E1770" t="s">
+        <v>6362</v>
       </c>
     </row>
     <row r="1771" spans="1:5" x14ac:dyDescent="0.2">
@@ -43913,9 +43960,8 @@
       <c r="C1771" t="s">
         <v>6347</v>
       </c>
-      <c r="E1771" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_ipc_memory_handle_new (const guint8 *data,    gsize size,    GError **error);;GArrowCUDAIPCMemoryHandle *</v>
+      <c r="E1771" t="s">
+        <v>6363</v>
       </c>
     </row>
     <row r="1772" spans="1:5" x14ac:dyDescent="0.2">
@@ -43928,9 +43974,8 @@
       <c r="C1772" t="s">
         <v>6348</v>
       </c>
-      <c r="E1772" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_ipc_memory_handle_serialize(GArrowCUDAIPCMemoryHandle *handle, GError **error);;GArrowBuffer *</v>
+      <c r="E1772" t="s">
+        <v>6364</v>
       </c>
     </row>
     <row r="1773" spans="1:5" x14ac:dyDescent="0.2">
@@ -43943,9 +43988,8 @@
       <c r="C1773" t="s">
         <v>6332</v>
       </c>
-      <c r="E1773" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_input_stream_new (GArrowCUDABuffer *buffer);;GArrowCUDABufferInputStream *</v>
+      <c r="E1773" t="s">
+        <v>6365</v>
       </c>
     </row>
     <row r="1774" spans="1:5" x14ac:dyDescent="0.2">
@@ -43958,9 +44002,8 @@
       <c r="C1774" t="s">
         <v>6333</v>
       </c>
-      <c r="E1774" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_output_stream_new (GArrowCUDABuffer *buffer);;GArrowCUDABufferOutputStream *</v>
+      <c r="E1774" t="s">
+        <v>6366</v>
       </c>
     </row>
     <row r="1775" spans="1:5" x14ac:dyDescent="0.2">
@@ -43973,9 +44016,8 @@
       <c r="C1775" t="s">
         <v>6349</v>
       </c>
-      <c r="E1775" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_output_stream_set_buffer_size(GArrowCUDABufferOutputStream *stream, gint64 size, GError **error);;gboolean</v>
+      <c r="E1775" t="s">
+        <v>6367</v>
       </c>
     </row>
     <row r="1776" spans="1:5" x14ac:dyDescent="0.2">
@@ -43988,9 +44030,8 @@
       <c r="C1776" t="s">
         <v>6336</v>
       </c>
-      <c r="E1776" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_output_stream_get_buffer_size(GArrowCUDABufferOutputStream *stream);;gint64</v>
+      <c r="E1776" t="s">
+        <v>6368</v>
       </c>
     </row>
     <row r="1777" spans="1:5" x14ac:dyDescent="0.2">
@@ -44003,9 +44044,8 @@
       <c r="C1777" t="s">
         <v>6337</v>
       </c>
-      <c r="E1777" t="str">
-        <f t="shared" si="0"/>
-        <v>garrow_cuda_buffer_output_stream_get_buffered_size(GArrowCUDABufferOutputStream *stream);;gint64</v>
+      <c r="E1777" t="s">
+        <v>6369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>